<commit_message>
Modified test file to have a date (rather than just a string)
</commit_message>
<xml_diff>
--- a/tests/files/simple.xlsx
+++ b/tests/files/simple.xlsx
@@ -5,153 +5,156 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="input-valid" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
-  <si>
-    <t>Qué?</t>
-  </si>
-  <si>
-    <t>Quién?</t>
-  </si>
-  <si>
-    <t>Para quién?</t>
-  </si>
-  <si>
-    <t>Dónde?</t>
-  </si>
-  <si>
-    <t>Cuándo?</t>
-  </si>
-  <si>
-    <t>Registro</t>
-  </si>
-  <si>
-    <t>Sector/Cluster</t>
-  </si>
-  <si>
-    <t>Subsector</t>
-  </si>
-  <si>
-    <t>Organización</t>
-  </si>
-  <si>
-    <t>Hombres</t>
-  </si>
-  <si>
-    <t>Mujeres</t>
-  </si>
-  <si>
-    <t>País</t>
-  </si>
-  <si>
-    <t>Departamento/Provincia/Estado</t>
-  </si>
-  <si>
-    <t>#sector+es</t>
-  </si>
-  <si>
-    <t>#subsector+es</t>
-  </si>
-  <si>
-    <t>#org+es</t>
-  </si>
-  <si>
-    <t>#targeted+f</t>
-  </si>
-  <si>
-    <t>#targeted+m</t>
-  </si>
-  <si>
-    <t>#country</t>
-  </si>
-  <si>
-    <t>#adm1</t>
-  </si>
-  <si>
-    <t>#date+reported</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>WASH</t>
-  </si>
-  <si>
-    <t>Higiene</t>
-  </si>
-  <si>
-    <t>ACNUR</t>
-  </si>
-  <si>
-    <t>Panamá</t>
-  </si>
-  <si>
-    <t>Los Santos</t>
-  </si>
-  <si>
-    <t>1 March 2015</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>Salud</t>
-  </si>
-  <si>
-    <t>Vacunación</t>
-  </si>
-  <si>
-    <t>OMS</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>Cauca</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>Educación</t>
-  </si>
-  <si>
-    <t>Formación de enseñadores</t>
-  </si>
-  <si>
-    <t>UNICEF</t>
-  </si>
-  <si>
-    <t>Chocó</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>Urbano</t>
-  </si>
-  <si>
-    <t>Venezuela</t>
-  </si>
-  <si>
-    <t>Amazonas</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+  <si>
+    <t xml:space="preserve">Qué?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quién?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para quién?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dónde?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuándo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector/Cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organización</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hombres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mujeres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">País</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Departamento/Provincia/Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#sector+es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#subsector+es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#org+es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#targeted+f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#targeted+m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#adm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#date+reported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Higiene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACNUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panamá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vacunación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colombia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cauca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formación de enseñadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chocó</t>
+  </si>
+  <si>
+    <t xml:space="preserve">004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urbano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venezuela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazonas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mmm\ d&quot;, &quot;yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -232,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -249,43 +252,46 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.1581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.90816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,10 +310,10 @@
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -388,42 +394,42 @@
       <c r="H4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>27</v>
+      <c r="I4" s="4" t="n">
+        <v>42064</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>250</v>
@@ -432,24 +438,24 @@
         <v>300</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>80</v>
@@ -458,21 +464,21 @@
         <v>95</v>
       </c>
       <c r="G7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Fill in any missing rows.
</commit_message>
<xml_diff>
--- a/tests/files/simple.xlsx
+++ b/tests/files/simple.xlsx
@@ -273,24 +273,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.65"/>
   </cols>
   <sheetData>
@@ -307,10 +305,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
@@ -444,29 +442,29 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F8" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>